<commit_message>
Updated examples to ViS format. Added .xls
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_run0805\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\Privatist\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,25 +24,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Personid</t>
-  </si>
-  <si>
-    <t>Fullstendig navn</t>
-  </si>
-  <si>
-    <t>Etternavn, Fornavn</t>
-  </si>
-  <si>
-    <t>Fornavn, Etternavn</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Eksamensparti</t>
+  </si>
+  <si>
+    <t>Eksamensdato</t>
+  </si>
+  <si>
+    <t>Fødselsnummer</t>
+  </si>
+  <si>
+    <t>MAT1001-1-E</t>
+  </si>
+  <si>
+    <t>17.11.2021</t>
+  </si>
+  <si>
+    <t>PSP5734-1-E</t>
+  </si>
+  <si>
+    <t>18.11.2021</t>
+  </si>
+  <si>
+    <t>01234567890</t>
+  </si>
+  <si>
+    <t>01234567891</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +65,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -67,12 +105,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,41 +422,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1234567890</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1234567891</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>